<commit_message>
Updated example hyperlink file
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/Hyperlinks.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/Hyperlinks.xlsx
@@ -35,19 +35,19 @@
     <x:t>Link to an address in this worksheet</x:t>
   </x:si>
   <x:si>
+    <x:t>Link to a range in this worksheet</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Link to an email message</x:t>
+  </x:si>
+  <x:si>
+    <x:t>This is no longer a link</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Odd looking link</x:t>
+  </x:si>
+  <x:si>
     <x:t>Link to an address in another worksheet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Link to a range in this worksheet</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Link to an email message</x:t>
-  </x:si>
-  <x:si>
-    <x:t>This is no longer a link</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Odd looking link</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -428,13 +428,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A13"/>
+  <x:dimension ref="A1:A14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="37.750625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="55.700625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:1">
@@ -478,34 +478,40 @@
       </x:c>
     </x:row>
     <x:row r="9" spans="1:1">
-      <x:c r="A9" s="1" t="s">
+      <x:c r="A9" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:1">
-      <x:c r="A10" s="0" t="s">
+      <x:c r="A10" s="2" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:1">
-      <x:c r="A11" s="2" t="s">
+      <x:c r="A11" s="1" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1"/>
+    <x:row r="12" spans="1:1">
+      <x:c r="A12" s="1">
+        <x:f>HYPERLINK("mailto:test@test.com", "Send Email")</x:f>
+      </x:c>
+    </x:row>
     <x:row r="13" spans="1:1"/>
+    <x:row r="14" spans="1:1"/>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="A1" r:id="rId11"/>
-    <x:hyperlink ref="A2" r:id="rId13" tooltip="Click to go to Yahoo!"/>
+    <x:hyperlink ref="A1" r:id="rId14"/>
+    <x:hyperlink ref="A2" r:id="rId15" tooltip="Click to go to Yahoo!"/>
     <x:hyperlink ref="A3" location="'Hyperlinks'!Test.xlsx" display="Link to a file - same folder"/>
-    <x:hyperlink ref="A4" r:id="rId14"/>
-    <x:hyperlink ref="A5" r:id="rId15"/>
+    <x:hyperlink ref="A4" r:id="rId16"/>
+    <x:hyperlink ref="A5" r:id="rId17"/>
     <x:hyperlink ref="A6" location="'Hyperlinks'!B1" display="Link to an address in this worksheet"/>
-    <x:hyperlink ref="A7" location="'Second Sheet'!A1" display="Link to an address in another worksheet"/>
-    <x:hyperlink ref="A8" location="'Hyperlinks'!B1:C2" tooltip="SquareBox" display="Link to a range in this worksheet"/>
-    <x:hyperlink ref="A9" r:id="rId16"/>
-    <x:hyperlink ref="A11" location="'Hyperlinks'!B1:C2" display="Odd looking link"/>
+    <x:hyperlink ref="A7" location="'Hyperlinks'!B1:C2" tooltip="SquareBox" display="Link to a range in this worksheet"/>
+    <x:hyperlink ref="A8" r:id="rId18"/>
+    <x:hyperlink ref="A10" location="'Hyperlinks'!B1:C2" display="Odd looking link"/>
+    <x:hyperlink ref="A11" location="'Second Sheet'!A1" display="Link to an address in another worksheet"/>
+    <x:hyperlink ref="A12" r:id="rId19" tooltip="'Send Email'"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Add extension method to wrap sheet name in quotes, only if required, i.e. it contains a space in the name Throw exception of invalid named range is added on workbook scope Contain named range references to minimum and maximum column and row dimensions when deleting rows / columns. Fixes #328
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/Hyperlinks.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/Hyperlinks.xlsx
@@ -503,14 +503,14 @@
   <x:hyperlinks>
     <x:hyperlink ref="A1" r:id="rId14"/>
     <x:hyperlink ref="A2" r:id="rId15" tooltip="Click to go to Yahoo!"/>
-    <x:hyperlink ref="A3" location="'Hyperlinks'!Test.xlsx" display="Link to a file - same folder"/>
+    <x:hyperlink ref="A3" location="Hyperlinks!Test.xlsx" display="Link to a file - same folder"/>
     <x:hyperlink ref="A4" r:id="rId16"/>
     <x:hyperlink ref="A5" r:id="rId17"/>
-    <x:hyperlink ref="A6" location="'Hyperlinks'!B1" display="Link to an address in this worksheet"/>
+    <x:hyperlink ref="A6" location="Hyperlinks!B1" display="Link to an address in this worksheet"/>
     <x:hyperlink ref="A7" location="'Second Sheet'!A1" display="Link to an address in another worksheet"/>
-    <x:hyperlink ref="A8" location="'Hyperlinks'!B1:C2" tooltip="SquareBox" display="Link to a range in this worksheet"/>
+    <x:hyperlink ref="A8" location="Hyperlinks!B1:C2" tooltip="SquareBox" display="Link to a range in this worksheet"/>
     <x:hyperlink ref="A9" r:id="rId18"/>
-    <x:hyperlink ref="A11" location="'Hyperlinks'!B1:C2" display="Odd looking link"/>
+    <x:hyperlink ref="A11" location="Hyperlinks!B1:C2" display="Odd looking link"/>
     <x:hyperlink ref="A12" r:id="rId19" tooltip="'Send Email'"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>